<commit_message>
added api endpoints for receiving post requests
</commit_message>
<xml_diff>
--- a/DEWSapp/dewsdocs/DATAitcz10.xlsx
+++ b/DEWSapp/dewsdocs/DATAitcz10.xlsx
@@ -2719,20 +2719,128 @@
       <c r="B56" t="n">
         <v>2.6</v>
       </c>
+      <c r="C56" t="n">
+        <v>3.27</v>
+      </c>
+      <c r="D56" t="n">
+        <v>4.68</v>
+      </c>
+      <c r="E56" t="n">
+        <v>8.91</v>
+      </c>
+      <c r="F56" t="n">
+        <v>10.01</v>
+      </c>
+      <c r="G56" t="n">
+        <v>10.93</v>
+      </c>
+      <c r="H56" t="n">
+        <v>15.16</v>
+      </c>
+      <c r="I56" t="n">
+        <v>13.86</v>
+      </c>
+      <c r="J56" t="n">
+        <v>9.59</v>
+      </c>
+      <c r="K56" t="n">
+        <v>9.56</v>
+      </c>
+      <c r="L56" t="n">
+        <v>7.94</v>
+      </c>
+      <c r="M56" t="n">
+        <v>2.53</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
         <v>2026</v>
       </c>
+      <c r="B57" t="n">
+        <v>5.07</v>
+      </c>
+      <c r="C57" t="n">
+        <v>4.78</v>
+      </c>
+      <c r="D57" t="n">
+        <v>4.33</v>
+      </c>
+      <c r="E57" t="n">
+        <v>4.67</v>
+      </c>
+      <c r="F57" t="n">
+        <v>8.470000000000001</v>
+      </c>
+      <c r="G57" t="n">
+        <v>9.34</v>
+      </c>
+      <c r="H57" t="n">
+        <v>15.92</v>
+      </c>
+      <c r="I57" t="n">
+        <v>13.89</v>
+      </c>
+      <c r="J57" t="n">
+        <v>12.8</v>
+      </c>
+      <c r="K57" t="n">
+        <v>7.41</v>
+      </c>
+      <c r="L57" t="n">
+        <v>4.97</v>
+      </c>
+      <c r="M57" t="n">
+        <v>3.14</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
         <v>2027</v>
       </c>
+      <c r="B58" t="n">
+        <v>0.95</v>
+      </c>
+      <c r="C58" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="D58" t="n">
+        <v>3.11</v>
+      </c>
+      <c r="E58" t="n">
+        <v>7.39</v>
+      </c>
+      <c r="F58" t="n">
+        <v>7.98</v>
+      </c>
+      <c r="G58" t="n">
+        <v>11.72</v>
+      </c>
+      <c r="H58" t="n">
+        <v>10.63</v>
+      </c>
+      <c r="I58" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="J58" t="n">
+        <v>12.65</v>
+      </c>
+      <c r="K58" t="n">
+        <v>8.85</v>
+      </c>
+      <c r="L58" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="M58" t="n">
+        <v>3.23</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
         <v>2028</v>
+      </c>
+      <c r="B59" t="n">
+        <v>6.21</v>
       </c>
     </row>
     <row r="60">

</xml_diff>

<commit_message>
adjusted path to excel file
</commit_message>
<xml_diff>
--- a/DEWSapp/dewsdocs/DATAitcz10.xlsx
+++ b/DEWSapp/dewsdocs/DATAitcz10.xlsx
@@ -2553,7 +2553,7 @@
         <v>2021</v>
       </c>
       <c r="B52" t="n">
-        <v>1.51595653928924</v>
+        <v>1.52</v>
       </c>
       <c r="C52" t="n">
         <v>0.9152444075799757</v>
@@ -2842,20 +2842,137 @@
       <c r="B59" t="n">
         <v>6.21</v>
       </c>
+      <c r="C59" t="n">
+        <v>2.18</v>
+      </c>
+      <c r="D59" t="n">
+        <v>2.61</v>
+      </c>
+      <c r="E59" t="n">
+        <v>5.65</v>
+      </c>
+      <c r="F59" t="n">
+        <v>10.47</v>
+      </c>
+      <c r="G59" t="n">
+        <v>13.22</v>
+      </c>
+      <c r="H59" t="n">
+        <v>14.03</v>
+      </c>
+      <c r="I59" t="n">
+        <v>13.52</v>
+      </c>
+      <c r="J59" t="n">
+        <v>10.26</v>
+      </c>
+      <c r="K59" t="n">
+        <v>7.26</v>
+      </c>
+      <c r="L59" t="n">
+        <v>10.11</v>
+      </c>
+      <c r="M59" t="n">
+        <v>1.12</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
         <v>2029</v>
       </c>
+      <c r="B60" t="n">
+        <v>1.87</v>
+      </c>
+      <c r="C60" t="n">
+        <v>2.53</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.97</v>
+      </c>
+      <c r="E60" t="n">
+        <v>5.29</v>
+      </c>
+      <c r="F60" t="n">
+        <v>10</v>
+      </c>
+      <c r="G60" t="n">
+        <v>10.99</v>
+      </c>
+      <c r="H60" t="n">
+        <v>10.93</v>
+      </c>
+      <c r="I60" t="n">
+        <v>13.26</v>
+      </c>
+      <c r="J60" t="n">
+        <v>12.15</v>
+      </c>
+      <c r="K60" t="n">
+        <v>11.15</v>
+      </c>
+      <c r="L60" t="n">
+        <v>6.85</v>
+      </c>
+      <c r="M60" t="n">
+        <v>1.3</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
         <v>2030</v>
       </c>
+      <c r="B61" t="n">
+        <v>2.77</v>
+      </c>
+      <c r="C61" t="n">
+        <v>3.36</v>
+      </c>
+      <c r="D61" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="E61" t="n">
+        <v>2.95</v>
+      </c>
+      <c r="F61" t="n">
+        <v>8.800000000000001</v>
+      </c>
+      <c r="G61" t="n">
+        <v>12.33</v>
+      </c>
+      <c r="H61" t="n">
+        <v>12.35</v>
+      </c>
+      <c r="I61" t="n">
+        <v>14.54</v>
+      </c>
+      <c r="J61" t="n">
+        <v>10.39</v>
+      </c>
+      <c r="K61" t="n">
+        <v>8.42</v>
+      </c>
+      <c r="L61" t="n">
+        <v>5.71</v>
+      </c>
+      <c r="M61" t="n">
+        <v>3.87</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
         <v>2031</v>
+      </c>
+      <c r="B62" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="C62" t="n">
+        <v>2.79</v>
+      </c>
+      <c r="D62" t="n">
+        <v>3.04</v>
+      </c>
+      <c r="E62" t="n">
+        <v>4.08</v>
       </c>
     </row>
     <row r="63">

</xml_diff>